<commit_message>
HIPPO ahora si completito
</commit_message>
<xml_diff>
--- a/Ex/Testing/HIPPO_test/result/results_HIPPO.xlsx
+++ b/Ex/Testing/HIPPO_test/result/results_HIPPO.xlsx
@@ -13,28 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>FFF</t>
-  </si>
-  <si>
-    <t>Fobj</t>
-  </si>
-  <si>
-    <t>CCc</t>
-  </si>
-  <si>
-    <t>Akaike</t>
-  </si>
-  <si>
-    <t>BIC</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>I955</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>FFF</t>
   </si>
@@ -100,7 +79,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G15"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="true"/>
@@ -114,25 +93,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
@@ -140,19 +119,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>0.19721843623083418</v>
+        <v>0.20435211317939678</v>
       </c>
       <c r="C2" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="0">
-        <v>-24.972403287604322</v>
+        <v>-24.439413937203113</v>
       </c>
       <c r="E2" s="0">
-        <v>18.969499303461095</v>
+        <v>18.969974881927431</v>
       </c>
       <c r="F2" s="0">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G2" s="0">
         <v>1</v>
@@ -163,19 +142,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>0.1972355844776984</v>
+        <v>0.20435219629732818</v>
       </c>
       <c r="C3" s="0">
         <v>1</v>
       </c>
       <c r="D3" s="0">
-        <v>-34.971099082872669</v>
+        <v>-34.439407836122484</v>
       </c>
       <c r="E3" s="0">
-        <v>16.261450245578441</v>
+        <v>16.261924686366413</v>
       </c>
       <c r="F3" s="0">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G3" s="0">
         <v>1</v>
@@ -186,19 +165,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>0.19721852518222022</v>
+        <v>0.20435271597815149</v>
       </c>
       <c r="C4" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="0">
-        <v>-34.972396518625345</v>
+        <v>-34.439369690202938</v>
       </c>
       <c r="E4" s="0">
-        <v>16.261449108292073</v>
+        <v>16.261924721011802</v>
       </c>
       <c r="F4" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G4" s="0">
         <v>1</v>
@@ -209,19 +188,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>0.19721849447103051</v>
+        <v>0.20435446443291755</v>
       </c>
       <c r="C5" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>-34.972398854449949</v>
+        <v>-34.439241349803041</v>
       </c>
       <c r="E5" s="0">
-        <v>16.261449106244662</v>
+        <v>16.261924837575453</v>
       </c>
       <c r="F5" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G5" s="0">
         <v>1</v>
@@ -232,19 +211,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>0.1972186218254991</v>
+        <v>0.20435188182735609</v>
       </c>
       <c r="C6" s="0">
         <v>1</v>
       </c>
       <c r="D6" s="0">
-        <v>-42.472389168155473</v>
+        <v>-41.939430919080706</v>
       </c>
       <c r="E6" s="0">
-        <v>13.553398913632751</v>
+        <v>13.553874464299541</v>
       </c>
       <c r="F6" s="0">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G6" s="0">
         <v>1</v>
@@ -255,19 +234,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>0.19721835487498537</v>
+        <v>0.20435279759697383</v>
       </c>
       <c r="C7" s="0">
         <v>1</v>
       </c>
       <c r="D7" s="0">
-        <v>-42.472409472383632</v>
+        <v>-41.939363699178628</v>
       </c>
       <c r="E7" s="0">
-        <v>13.553398895835555</v>
+        <v>13.553874525350849</v>
       </c>
       <c r="F7" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G7" s="0">
         <v>1</v>
@@ -278,19 +257,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>0.19721844700355423</v>
+        <v>0.20435186502898034</v>
       </c>
       <c r="C8" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="0">
-        <v>-42.472402464721043</v>
+        <v>-41.93943215212856</v>
       </c>
       <c r="E8" s="0">
-        <v>13.553398901977955</v>
+        <v>13.55387446317965</v>
       </c>
       <c r="F8" s="0">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G8" s="0">
         <v>1</v>
@@ -301,21 +280,159 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>0.19721815139243926</v>
+        <v>0.20435187577887123</v>
       </c>
       <c r="C9" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="0">
-        <v>-48.305758281600497</v>
+        <v>-41.939431363056428</v>
       </c>
       <c r="E9" s="0">
-        <v>10.845348681168336</v>
+        <v>13.553874463896308</v>
       </c>
       <c r="F9" s="0">
+        <v>14</v>
+      </c>
+      <c r="G9" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0">
+        <v>0.2043533037566907</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0">
+        <v>-41.939326545851443</v>
+      </c>
+      <c r="E10" s="0">
+        <v>13.55387455909483</v>
+      </c>
+      <c r="F10" s="0">
+        <v>13</v>
+      </c>
+      <c r="G10" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0">
+        <v>0.20435244448880252</v>
+      </c>
+      <c r="C11" s="0">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0">
+        <v>-47.77272295154615</v>
+      </c>
+      <c r="E11" s="0">
+        <v>10.845824300708093</v>
+      </c>
+      <c r="F11" s="0">
         <v>12</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G11" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0">
+        <v>0.20435191503010858</v>
+      </c>
+      <c r="C12" s="0">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0">
+        <v>-47.772761815239299</v>
+      </c>
+      <c r="E12" s="0">
+        <v>10.845824265410847</v>
+      </c>
+      <c r="F12" s="0">
+        <v>13</v>
+      </c>
+      <c r="G12" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0">
+        <v>0.20435201099124234</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0">
+        <v>-47.772754771426328</v>
+      </c>
+      <c r="E13" s="0">
+        <v>10.845824271808256</v>
+      </c>
+      <c r="F13" s="0">
+        <v>12</v>
+      </c>
+      <c r="G13" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0">
+        <v>0.20435353957786556</v>
+      </c>
+      <c r="C14" s="0">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0">
+        <v>-47.772642569381041</v>
+      </c>
+      <c r="E14" s="0">
+        <v>10.845824373714031</v>
+      </c>
+      <c r="F14" s="0">
+        <v>7</v>
+      </c>
+      <c r="G14" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0">
+        <v>0.20435214240639388</v>
+      </c>
+      <c r="C15" s="0">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0">
+        <v>-52.439411791862312</v>
+      </c>
+      <c r="E15" s="0">
+        <v>8.1377740794670554</v>
+      </c>
+      <c r="F15" s="0">
+        <v>6</v>
+      </c>
+      <c r="G15" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>